<commit_message>
new OBJ files, results
</commit_message>
<xml_diff>
--- a/metaData.xlsx
+++ b/metaData.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="3750"/>
   </bookViews>
   <sheets>
-    <sheet name="metaData" sheetId="1" r:id="rId1"/>
+    <sheet name="metaData1" sheetId="2" r:id="rId1"/>
+    <sheet name="metaData" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>lookfrom</t>
   </si>
@@ -61,6 +62,12 @@
   </si>
   <si>
     <t>Rh_Narpa_z750.png</t>
+  </si>
+  <si>
+    <t>[0 -4 795]</t>
+  </si>
+  <si>
+    <t>[0 0 795]</t>
   </si>
 </sst>
 </file>
@@ -870,17 +877,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -897,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -914,7 +921,78 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
modified functions, plots, results
</commit_message>
<xml_diff>
--- a/metaData.xlsx
+++ b/metaData.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="3750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="3750" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="metaData1" sheetId="2" r:id="rId1"/>
-    <sheet name="metaData" sheetId="1" r:id="rId2"/>
+    <sheet name="metaData" sheetId="1" r:id="rId1"/>
+    <sheet name="metaData1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>lookfrom</t>
   </si>
@@ -64,10 +64,16 @@
     <t>Rh_Narpa_z750.png</t>
   </si>
   <si>
-    <t>[0 -4 795]</t>
-  </si>
-  <si>
-    <t>[0 0 795]</t>
+    <t>[0 -10 790]</t>
+  </si>
+  <si>
+    <t>Rh_Narpa_z790.png</t>
+  </si>
+  <si>
+    <t>rh_narpa_z790.txt</t>
+  </si>
+  <si>
+    <t>[0 -10 0]</t>
   </si>
 </sst>
 </file>
@@ -876,18 +882,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -921,12 +927,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -947,18 +953,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -992,21 +998,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>